<commit_message>
:up: ultimo commit antes de iniciar a leitura de pdf automatica
</commit_message>
<xml_diff>
--- a/banco_de_dados/metadados.xlsx
+++ b/banco_de_dados/metadados.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,34 @@
       <c r="A5" t="inlineStr">
         <is>
           <t>Caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>UNIRIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Liquigás</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>BNDES</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CEFET-RJ</t>
         </is>
       </c>
     </row>
@@ -606,7 +634,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -661,6 +689,96 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Acentos Diferenciais</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ortografia Oficial</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Emprego do Hífen</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Expressões Problemáticas</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Substantivo</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Adjetivo</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
:up: adicionado efeito de carregamentos
</commit_message>
<xml_diff>
--- a/banco_de_dados/metadados.xlsx
+++ b/banco_de_dados/metadados.xlsx
@@ -634,7 +634,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -779,6 +779,21 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Conjunção</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Português</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>